<commit_message>
filled out scrum sheet with tasks for sprint 4
</commit_message>
<xml_diff>
--- a/P10/store/Scrum.xlsx
+++ b/P10/store/Scrum.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P10/store/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ACB9AB8-D097-874D-9D78-7D74761980C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08DE776-14D4-5449-B062-6844B8C4DEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="201">
   <si>
     <t>Product Name:</t>
   </si>
@@ -615,6 +615,36 @@
   </si>
   <si>
     <t>Write the onOpenClick method in MainWin.java</t>
+  </si>
+  <si>
+    <t>In Work</t>
+  </si>
+  <si>
+    <t>in gui.MainWin, add Order to the Insert menu + button on toolbar</t>
+  </si>
+  <si>
+    <t>write method onInsertOrderClick()</t>
+  </si>
+  <si>
+    <t>implement the ActionListener to call onInsertOrderClick()</t>
+  </si>
+  <si>
+    <t>update store.Order to add the cost() method</t>
+  </si>
+  <si>
+    <t>include the cost() in Order.toString()</t>
+  </si>
+  <si>
+    <t>in gui.MainWin, add Orders to the View menu + button on toolbar</t>
+  </si>
+  <si>
+    <t>implement the ActionListener to display all Orders</t>
+  </si>
+  <si>
+    <t>Implement custom dialogs when adding customer, option, computer</t>
+  </si>
+  <si>
+    <t>update the About dialog + check File I/O code still works</t>
   </si>
 </sst>
 </file>
@@ -897,6 +927,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -911,12 +947,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2301,7 +2331,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -2379,28 +2409,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2450,7 +2480,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -2524,7 +2554,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -3813,8 +3843,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="141" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView topLeftCell="A31" zoomScale="141" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3837,14 +3867,14 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="47" t="s">
         <v>157</v>
       </c>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
       <c r="H1" s="5"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
@@ -3855,14 +3885,14 @@
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="46">
+      <c r="B2" s="48">
         <v>243</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -3901,66 +3931,66 @@
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="47" t="s">
+      <c r="B5" s="49" t="s">
         <v>158</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
       <c r="H5" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I5" s="49">
+      <c r="I5" s="44">
         <v>1001730963</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A6"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A7"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
+      <c r="B7" s="45"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="45"/>
+      <c r="E7" s="45"/>
+      <c r="F7" s="45"/>
+      <c r="G7" s="45"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
+      <c r="B8" s="45"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A9"/>
-      <c r="B9" s="43"/>
-      <c r="C9" s="43"/>
-      <c r="D9" s="43"/>
-      <c r="E9" s="43"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="43"/>
+      <c r="B9" s="45"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
@@ -4188,10 +4218,10 @@
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="44" t="s">
+      <c r="F22" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="44"/>
+      <c r="G22" s="46"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13" t="s">
         <v>19</v>
@@ -4801,7 +4831,9 @@
       <c r="F41" s="17">
         <v>4</v>
       </c>
-      <c r="G41" s="17"/>
+      <c r="G41" s="17" t="s">
+        <v>191</v>
+      </c>
       <c r="H41" s="18" t="s">
         <v>31</v>
       </c>
@@ -4830,7 +4862,9 @@
       <c r="F42" s="17">
         <v>4</v>
       </c>
-      <c r="G42" s="17"/>
+      <c r="G42" s="17" t="s">
+        <v>191</v>
+      </c>
       <c r="H42" s="18" t="s">
         <v>31</v>
       </c>
@@ -4859,7 +4893,9 @@
       <c r="F43" s="17">
         <v>4</v>
       </c>
-      <c r="G43" s="17"/>
+      <c r="G43" s="17" t="s">
+        <v>191</v>
+      </c>
       <c r="H43" s="18" t="s">
         <v>31</v>
       </c>
@@ -4890,7 +4926,9 @@
       <c r="F44" s="17">
         <v>4</v>
       </c>
-      <c r="G44" s="17"/>
+      <c r="G44" s="17" t="s">
+        <v>191</v>
+      </c>
       <c r="H44" s="18" t="s">
         <v>31</v>
       </c>
@@ -6103,7 +6141,7 @@
         <v>30</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="43" t="s">
         <v>163</v>
       </c>
       <c r="E17" s="37" t="s">
@@ -7343,7 +7381,7 @@
         <v>49</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="43" t="s">
         <v>173</v>
       </c>
       <c r="E17" s="37" t="s">
@@ -8565,7 +8603,7 @@
         <v>74</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="48" t="s">
+      <c r="D17" s="43" t="s">
         <v>183</v>
       </c>
       <c r="E17" s="37" t="s">
@@ -9502,8 +9540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9607,7 +9645,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -9622,7 +9660,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -9640,7 +9678,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -9658,7 +9696,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -9676,7 +9714,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -9694,7 +9732,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -9712,7 +9750,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -9730,7 +9768,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -9776,91 +9814,125 @@
       <c r="A17" s="4">
         <v>1</v>
       </c>
-      <c r="B17" s="35"/>
+      <c r="B17" s="35" t="s">
+        <v>92</v>
+      </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="36" t="s">
-        <v>153</v>
+      <c r="D17" s="43" t="s">
+        <v>192</v>
       </c>
       <c r="E17" s="37"/>
       <c r="F17" s="38"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="4">
         <v>2</v>
       </c>
-      <c r="B18" s="35"/>
+      <c r="B18" s="35" t="s">
+        <v>92</v>
+      </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="39"/>
+      <c r="D18" s="39" t="s">
+        <v>193</v>
+      </c>
       <c r="E18" s="37"/>
       <c r="F18" s="38"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="4">
         <v>3</v>
       </c>
-      <c r="B19" s="35"/>
+      <c r="B19" s="35" t="s">
+        <v>92</v>
+      </c>
       <c r="C19" s="4"/>
-      <c r="D19" s="39"/>
+      <c r="D19" s="39" t="s">
+        <v>194</v>
+      </c>
       <c r="E19" s="37"/>
       <c r="F19" s="38"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="4">
         <v>4</v>
       </c>
-      <c r="B20" s="35"/>
+      <c r="B20" s="35" t="s">
+        <v>94</v>
+      </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="39"/>
+      <c r="D20" s="39" t="s">
+        <v>195</v>
+      </c>
       <c r="E20" s="37"/>
       <c r="F20" s="38"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="35" t="s">
+        <v>94</v>
+      </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="39"/>
+      <c r="D21" s="39" t="s">
+        <v>196</v>
+      </c>
       <c r="E21" s="37"/>
       <c r="F21" s="38"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4">
         <v>6</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="35" t="s">
+        <v>97</v>
+      </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="39"/>
+      <c r="D22" s="39" t="s">
+        <v>197</v>
+      </c>
       <c r="E22" s="37"/>
       <c r="F22" s="38"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="35" t="s">
+        <v>97</v>
+      </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="39"/>
+      <c r="D23" s="39" t="s">
+        <v>198</v>
+      </c>
       <c r="E23" s="37"/>
       <c r="F23" s="38"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4">
         <v>8</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="35" t="s">
+        <v>101</v>
+      </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="39"/>
+      <c r="D24" s="39" t="s">
+        <v>199</v>
+      </c>
       <c r="E24" s="37"/>
       <c r="F24" s="38"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="4">
         <v>9</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="35" t="s">
+        <v>101</v>
+      </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="39"/>
+      <c r="D25" s="39" t="s">
+        <v>200</v>
+      </c>
       <c r="E25" s="37"/>
       <c r="F25" s="38"/>
     </row>

</xml_diff>

<commit_message>
added buttons/icons for order + upadated about dialog
</commit_message>
<xml_diff>
--- a/P10/store/Scrum.xlsx
+++ b/P10/store/Scrum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P10/store/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08DE776-14D4-5449-B062-6844B8C4DEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCDCC70-152E-9046-A35B-0C9FE763EE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="202">
   <si>
     <t>Product Name:</t>
   </si>
@@ -645,6 +645,9 @@
   </si>
   <si>
     <t>update the About dialog + check File I/O code still works</t>
+  </si>
+  <si>
+    <t>In Test</t>
   </si>
 </sst>
 </file>
@@ -2424,13 +2427,13 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4832,7 +4835,7 @@
         <v>4</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="H41" s="18" t="s">
         <v>31</v>
@@ -4863,7 +4866,7 @@
         <v>4</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="H42" s="18" t="s">
         <v>31</v>
@@ -4894,7 +4897,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>191</v>
+        <v>201</v>
       </c>
       <c r="H43" s="18" t="s">
         <v>31</v>
@@ -9540,8 +9543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9732,11 +9735,11 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -9750,7 +9753,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -9768,7 +9771,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -9821,7 +9824,9 @@
       <c r="D17" s="43" t="s">
         <v>192</v>
       </c>
-      <c r="E17" s="37"/>
+      <c r="E17" s="37" t="s">
+        <v>172</v>
+      </c>
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -9835,7 +9840,9 @@
       <c r="D18" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="E18" s="37"/>
+      <c r="E18" s="37" t="s">
+        <v>191</v>
+      </c>
       <c r="F18" s="38"/>
     </row>
     <row r="19" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -9849,7 +9856,9 @@
       <c r="D19" s="39" t="s">
         <v>194</v>
       </c>
-      <c r="E19" s="37"/>
+      <c r="E19" s="37" t="s">
+        <v>172</v>
+      </c>
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -9863,7 +9872,9 @@
       <c r="D20" s="39" t="s">
         <v>195</v>
       </c>
-      <c r="E20" s="37"/>
+      <c r="E20" s="37" t="s">
+        <v>172</v>
+      </c>
       <c r="F20" s="38"/>
     </row>
     <row r="21" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -9877,7 +9888,9 @@
       <c r="D21" s="39" t="s">
         <v>196</v>
       </c>
-      <c r="E21" s="37"/>
+      <c r="E21" s="37" t="s">
+        <v>172</v>
+      </c>
       <c r="F21" s="38"/>
     </row>
     <row r="22" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -9891,7 +9904,9 @@
       <c r="D22" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="E22" s="37"/>
+      <c r="E22" s="37" t="s">
+        <v>172</v>
+      </c>
       <c r="F22" s="38"/>
     </row>
     <row r="23" spans="1:6" ht="14" x14ac:dyDescent="0.15">
@@ -9905,7 +9920,9 @@
       <c r="D23" s="39" t="s">
         <v>198</v>
       </c>
-      <c r="E23" s="37"/>
+      <c r="E23" s="37" t="s">
+        <v>172</v>
+      </c>
       <c r="F23" s="38"/>
     </row>
     <row r="24" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
finished implementation of method onInsertOrderClick() + updated scrum sheet
</commit_message>
<xml_diff>
--- a/P10/store/Scrum.xlsx
+++ b/P10/store/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P10/store/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCDCC70-152E-9046-A35B-0C9FE763EE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A57BB3-8783-FA46-9376-53B9249BAB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="202">
   <si>
     <t>Product Name:</t>
   </si>
@@ -647,7 +647,7 @@
     <t>update the About dialog + check File I/O code still works</t>
   </si>
   <si>
-    <t>In Test</t>
+    <t>Finished in Sprint 4</t>
   </si>
 </sst>
 </file>
@@ -1182,10 +1182,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2427,13 +2427,13 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3846,7 +3846,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ101"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="141" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="141" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
@@ -4129,11 +4129,11 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$107,"Finished in Sprint 4")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="5"/>
@@ -4149,11 +4149,11 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$107,"Finished in Sprint 4")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="5"/>
@@ -9543,8 +9543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9735,11 +9735,11 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D12" s="25"/>
       <c r="E12" s="25"/>
@@ -9753,7 +9753,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -9771,7 +9771,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -9841,7 +9841,7 @@
         <v>193</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="F18" s="38"/>
     </row>
@@ -9950,7 +9950,9 @@
       <c r="D25" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="E25" s="37"/>
+      <c r="E25" s="37" t="s">
+        <v>172</v>
+      </c>
       <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
finished for full credit + finished scrum sheet
</commit_message>
<xml_diff>
--- a/P10/store/Scrum.xlsx
+++ b/P10/store/Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcia/Desktop/cse1325/P10/store/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49A57BB3-8783-FA46-9376-53B9249BAB5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A114387-5E75-D843-971F-33959229575F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="15880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="202">
   <si>
     <t>Product Name:</t>
   </si>
@@ -617,9 +617,6 @@
     <t>Write the onOpenClick method in MainWin.java</t>
   </si>
   <si>
-    <t>In Work</t>
-  </si>
-  <si>
     <t>in gui.MainWin, add Order to the Insert menu + button on toolbar</t>
   </si>
   <si>
@@ -648,6 +645,9 @@
   </si>
   <si>
     <t>Finished in Sprint 4</t>
+  </si>
+  <si>
+    <t>Completed Day 6</t>
   </si>
 </sst>
 </file>
@@ -1182,10 +1182,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2430,10 +2430,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2648,7 +2648,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -2797,7 +2797,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -2871,7 +2871,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -2962,7 +2962,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -3111,7 +3111,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -3185,7 +3185,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -3846,7 +3846,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="141" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="141" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
@@ -4129,11 +4129,11 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$107,"Finished in Sprint 4")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="5"/>
@@ -4149,11 +4149,11 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$107,"Finished in Sprint 4")</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="5"/>
@@ -4835,7 +4835,7 @@
         <v>4</v>
       </c>
       <c r="G41" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H41" s="18" t="s">
         <v>31</v>
@@ -4866,7 +4866,7 @@
         <v>4</v>
       </c>
       <c r="G42" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H42" s="18" t="s">
         <v>31</v>
@@ -4897,7 +4897,7 @@
         <v>4</v>
       </c>
       <c r="G43" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H43" s="18" t="s">
         <v>31</v>
@@ -4930,7 +4930,7 @@
         <v>4</v>
       </c>
       <c r="G44" s="17" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="H44" s="18" t="s">
         <v>31</v>
@@ -9543,8 +9543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -9753,11 +9753,11 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
@@ -9771,7 +9771,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -9822,7 +9822,7 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="43" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E17" s="37" t="s">
         <v>172</v>
@@ -9838,7 +9838,7 @@
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="39" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E18" s="37" t="s">
         <v>172</v>
@@ -9854,7 +9854,7 @@
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="39" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E19" s="37" t="s">
         <v>172</v>
@@ -9870,7 +9870,7 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="39" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E20" s="37" t="s">
         <v>172</v>
@@ -9886,7 +9886,7 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="39" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E21" s="37" t="s">
         <v>172</v>
@@ -9902,7 +9902,7 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="39" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E22" s="37" t="s">
         <v>172</v>
@@ -9918,7 +9918,7 @@
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="39" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E23" s="37" t="s">
         <v>172</v>
@@ -9934,9 +9934,11 @@
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="39" t="s">
-        <v>199</v>
-      </c>
-      <c r="E24" s="37"/>
+        <v>198</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>201</v>
+      </c>
       <c r="F24" s="38"/>
     </row>
     <row r="25" spans="1:6" ht="14" customHeight="1" x14ac:dyDescent="0.15">
@@ -9948,7 +9950,7 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="39" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E25" s="37" t="s">
         <v>172</v>

</xml_diff>